<commit_message>
- Fixed Survey Option issue
</commit_message>
<xml_diff>
--- a/PlexByte.App.MoCap.Docs/DB Definition.xlsx
+++ b/PlexByte.App.MoCap.Docs/DB Definition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -3501,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
@@ -7141,9 +7141,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>